<commit_message>
Fixes to launch the browser
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -10,6 +10,8 @@
   <sheets>
     <sheet name="Index" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="facebook_Login_TC001" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="facebook_Login_TC002" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Demo_TC_TC003" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -47,16 +49,34 @@
     <t xml:space="preserve">facebook_Login_TC001</t>
   </si>
   <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify facebook login page with invalid credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facebook_Login_TC002</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Prod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify facebook login page with invalid credentials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smoke</t>
+    <t xml:space="preserve">Verify facebook SignUp page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demo_TC_TC003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What done is done when we say its done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dummy</t>
   </si>
   <si>
     <t xml:space="preserve">Username</t>
@@ -69,6 +89,15 @@
   </si>
   <si>
     <t xml:space="preserve">tony56432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Data</t>
   </si>
 </sst>
 </file>
@@ -198,10 +227,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -209,7 +238,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.32"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="7" style="0" width="11.51"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
@@ -253,6 +282,46 @@
       </c>
       <c r="F2" s="0" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -274,7 +343,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -285,18 +354,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -311,4 +380,96 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="C3:C4 C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="tonystark@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C4 A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>